<commit_message>
removed some debug text, updated tasklist table
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fb7b985650d8db8/Repositories/RevatureProject0/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7277559E-6B84-40B6-B5D0-94C62B30CB88}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
+    <workbookView xWindow="3795" yWindow="1170" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,9 +489,12 @@
       <c r="B3">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
       <c r="D3">
         <f t="shared" ref="D3:D12" si="0">IF(C3 = "DONE",B3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,7 +624,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ability for customers to post money transfer requests
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7277559E-6B84-40B6-B5D0-94C62B30CB88}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA46FE9D-7380-4D3E-B073-B09915E53E62}"/>
   <bookViews>
     <workbookView xWindow="3795" yWindow="1170" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,9 +582,12 @@
       <c r="B10">
         <v>3</v>
       </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,7 +627,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added user ability to approve or reject incumbent transfers, fixed a bug where incoming transfer request displayed requests already reponded to
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fb7b985650d8db8/Repositories/RevatureProject0/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA46FE9D-7380-4D3E-B073-B09915E53E62}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D31ADAA1-F922-4220-85EF-56F7551A5491}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="1170" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
+    <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,9 +597,12 @@
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +630,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ability for customers to make withdrawals
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fb7b985650d8db8/Repositories/RevatureProject0/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D31ADAA1-F922-4220-85EF-56F7551A5491}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F62608E6-9C16-4B1B-BB93-E405AC67F707}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add deposits for customers
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F62608E6-9C16-4B1B-BB93-E405AC67F707}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB569BAC-A2EC-44A5-A715-AFA2129CB768}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,9 +516,12 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,7 +633,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task list update, code cleanup in isle Main
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB569BAC-A2EC-44A5-A715-AFA2129CB768}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FEED7F07-B225-42C1-9F49-6A13043E6FE3}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,9 +531,12 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,7 +636,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added employee transaction viewer, updated task list appropriately
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FEED7F07-B225-42C1-9F49-6A13043E6FE3}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{665FC15D-F8C1-4D9B-B43F-C77CE0DA1F33}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,9 +618,12 @@
       <c r="B12">
         <v>2</v>
       </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +639,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
customers can now view summaries on all accounts, updated task list appropriately
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{665FC15D-F8C1-4D9B-B43F-C77CE0DA1F33}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A0683F1-3ADA-430E-9634-3F39BB3CC7A6}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,9 +504,12 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,7 +642,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Employees can now search for accounts by full name or account number, updated Task List
</commit_message>
<xml_diff>
--- a/Documentation/TaskStatus.xlsx
+++ b/Documentation/TaskStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\OneDrive\Repositories\RevatureProject0\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A0683F1-3ADA-430E-9634-3F39BB3CC7A6}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{47699134-34D8-4BA3-A7B4-5BBD9B547DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31DAFA06-5337-4A72-8397-12103ABC803A}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1860" windowWidth="18975" windowHeight="12885" xr2:uid="{513CF9E6-3706-4B69-B17D-9F9206D035BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>* As a customer, I can apply for a new bank account with a starting balance.</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,9 +564,12 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,7 +645,7 @@
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>